<commit_message>
updated docs with meeting notes
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28760" windowHeight="16340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="660" yWindow="460" windowWidth="28760" windowHeight="16340" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Meeting Notes" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="103">
   <si>
     <t xml:space="preserve">Date: </t>
   </si>
@@ -317,9 +317,6 @@
 - how does the suction pedal work? what is the plumbing?</t>
   </si>
   <si>
-    <t>- ear trimmers</t>
-  </si>
-  <si>
     <t>- goal: learning</t>
   </si>
   <si>
@@ -337,11 +334,6 @@
 </t>
   </si>
   <si>
-    <t>- remind Dr. James to share his surgery calendar when I get my badge/login
-- look up what to include in a time flow analysis
-- note which ears are hard to gain access of instruments</t>
-  </si>
-  <si>
     <t>General</t>
   </si>
   <si>
@@ -352,10 +344,6 @@
   </si>
   <si>
     <t>to be discussed with Dr. James</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - survey method: go on RedCap (formal SickKids survey/questionaire method) and formulate and send out the questionaire, use delphi method to figure out the criteria (time consuming) - requires many rounds of survey and group converges to the 'right' answer - this will take a long time but will have time to do, well defined method, more likelyhood of publication, audience will accept this method
-- nominal group method: quicker way to make the decision - many surgeons meet and vote/rank solutions in one meeting - could use this to figure out what questions to ask</t>
   </si>
   <si>
     <t>cleaning obstructed suction tool</t>
@@ -389,12 +377,98 @@
     <t xml:space="preserve">- obtain scan of the boy and make into 3D model 
 '- familiarize with software at CIGITI computer </t>
   </si>
+  <si>
+    <t xml:space="preserve">- ear trimmers - ordered 
+- </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- remind Dr. James to share his surgery calendar when I get my badge/login
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>- lliterature search for time flow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- note which ears are hard to gain access of instruments</t>
+    </r>
+  </si>
+  <si>
+    <t>time flow and questionaire</t>
+  </si>
+  <si>
+    <t>validation of instruments</t>
+  </si>
+  <si>
+    <t>in OR and in 3D printed model</t>
+  </si>
+  <si>
+    <t>- record time and number of changes to scissors</t>
+  </si>
+  <si>
+    <t>choosing committee</t>
+  </si>
+  <si>
+    <t>materials science and force required to choose the size of the tubing if using concentric tubes</t>
+  </si>
+  <si>
+    <t>what are the main technical hurdles that will take most time? - make a list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choosing size of tool - worskpace analysis and forces </t>
+  </si>
+  <si>
+    <t>mitacs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patent a modified instrument through sickkids </t>
+  </si>
+  <si>
+    <t>think about people who would be useful based on their experience/knowledge</t>
+  </si>
+  <si>
+    <t>- check about these requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - survey method: go on RedCap (formal SickKids survey/questionaire method) and formulate and send out the questionaire, use delphi method to figure out the criteria (time consuming) - requires many rounds of survey and group converges to the 'right' answer - this will take a long time but will have time to do, well defined method, more likelyhood of publication, audience will accept this method
+- nominal group method: quicker way to make the decision - many surgeons meet and vote/rank solutions in one meeting - could use this to figure out what questions to ask
+- quality function deployment - use matrices how well the design satisfies user's needs (look this up) - Jan has done this before, used in rehab engineering, can be used to design the questionaire and time flow study 
+- 6 months</t>
+  </si>
+  <si>
+    <t>structure of thesis?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isolate ear drum from CT scan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">print a model of the whole ear canal, scaled up 5X </t>
+  </si>
+  <si>
+    <t>how much to bend laser before fibres break</t>
+  </si>
+  <si>
+    <t>weld thomisin end effector onto a 19Fr suction tube, bend 19Fr sucker into same curvature as rosen and file it to sharpen the end and either put suction hole on the lateral or medial end.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -423,8 +497,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,6 +519,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF4185"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -553,6 +644,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -563,9 +672,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF4185"/>
       <color rgb="FF79F9C3"/>
       <color rgb="FFA58BFF"/>
-      <color rgb="FFFF4185"/>
     </mruColors>
   </colors>
   <extLst>
@@ -841,7 +950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -903,12 +1012,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J37"/>
+  <dimension ref="B1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -931,7 +1040,7 @@
         <v>27</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
@@ -1033,23 +1142,23 @@
     </row>
     <row r="11" spans="2:9" s="10" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="C11" s="11"/>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="24" t="s">
         <v>46</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="I11" s="12" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="2:9" s="13" customFormat="1" ht="128" x14ac:dyDescent="0.2">
       <c r="C12" s="14"/>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="25" t="s">
         <v>47</v>
       </c>
       <c r="F12" s="14"/>
@@ -1057,10 +1166,10 @@
         <v>66</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="32" x14ac:dyDescent="0.2">
@@ -1125,28 +1234,30 @@
       </c>
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="3:10" s="13" customFormat="1" ht="144" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:10" s="13" customFormat="1" ht="176" x14ac:dyDescent="0.2">
       <c r="C19" s="14"/>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="26" t="s">
         <v>48</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="14"/>
+      <c r="G19" s="14" t="s">
+        <v>85</v>
+      </c>
       <c r="H19" s="17" t="s">
         <v>59</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="3:10" s="13" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="C20" s="14"/>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="25" t="s">
         <v>39</v>
       </c>
       <c r="F20" s="14"/>
@@ -1181,11 +1292,11 @@
       <c r="I22" s="11"/>
     </row>
     <row r="23" spans="3:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="27" t="s">
         <v>38</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>49</v>
@@ -1203,12 +1314,12 @@
     </row>
     <row r="26" spans="3:10" ht="48" x14ac:dyDescent="0.2">
       <c r="I26" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="3:10" s="22" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="C30" s="21"/>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="28" t="s">
         <v>53</v>
       </c>
       <c r="F30" s="21"/>
@@ -1225,42 +1336,112 @@
         <v>57</v>
       </c>
     </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="I32" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
     <row r="34" spans="3:9" s="13" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="C34" s="14"/>
-      <c r="E34" s="14" t="s">
-        <v>82</v>
+      <c r="E34" s="25" t="s">
+        <v>79</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="3:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C35" s="21"/>
       <c r="E35" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
       <c r="I35" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.2">
       <c r="I36" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.2">
       <c r="E37" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E38" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="E39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="E40" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="E42" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E43" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E44" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E45" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="E46" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="E47" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" ht="64" x14ac:dyDescent="0.2">
+      <c r="E48" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1272,7 +1453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>